<commit_message>
View Search Strategy functionality
</commit_message>
<xml_diff>
--- a/Testdata/Non_Oncology/DataFiles/Protocol_Page/SearchStrategy/SearchStrategy_Nononco_Data.xlsx
+++ b/Testdata/Non_Oncology/DataFiles/Protocol_Page/SearchStrategy/SearchStrategy_Nononco_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\Non_Oncology\DataFiles\Protocol_Page\SearchStrategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B4DF8A-A464-495D-A0C9-9DD218EF5993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316E6879-BD5C-4C5E-8FF6-A80B15A76CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Economic</t>
   </si>
@@ -131,6 +131,21 @@
   </si>
   <si>
     <t>Real-world Evidence_search-strategy-template_Non-Oncology.xlsx</t>
+  </si>
+  <si>
+    <t>Population_Radio_button</t>
+  </si>
+  <si>
+    <t>LIVEHTA Automation - Test_NonOncology_Automation_3_radio_button</t>
+  </si>
+  <si>
+    <t>slrtype_Radio_button</t>
+  </si>
+  <si>
+    <t>Clinical_radio_button</t>
+  </si>
+  <si>
+    <t>pop2</t>
   </si>
 </sst>
 </file>
@@ -457,46 +472,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -504,99 +527,163 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>